<commit_message>
fix: edit database and edit admin
</commit_message>
<xml_diff>
--- a/font-end/admin/testExcel/danh_sach_nguoi_dung.xlsx.xlsx
+++ b/font-end/admin/testExcel/danh_sach_nguoi_dung.xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GITHUB\EduProjectSpace\font-end\admin\testExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF89A19-78BA-49A4-A4F6-A5798E962671}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A0A48D-247E-40FA-9D57-9485D33F45CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>nguyen.a@hutech.edu.vn</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Lê Văn Ca</t>
+  </si>
+  <si>
+    <t>21DTHA1</t>
   </si>
 </sst>
 </file>
@@ -360,21 +363,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>21520001</v>
       </c>
@@ -382,13 +384,16 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1">
-        <v>1</v>
+      <c r="E1">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>21520002</v>
       </c>
@@ -396,13 +401,16 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>2</v>
+      <c r="E2">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>21520004</v>
       </c>
@@ -410,9 +418,12 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>3</v>
       </c>
     </row>

</xml_diff>